<commit_message>
add week schedule use or
</commit_message>
<xml_diff>
--- a/staff.xlsx
+++ b/staff.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -28,55 +28,31 @@
     <t>Event Preference</t>
   </si>
   <si>
-    <t>Jackson J</t>
+    <t>Adam A</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Reception</t>
+  </si>
+  <si>
+    <t>Bob B</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
-    <t>Reception</t>
-  </si>
-  <si>
-    <t>Jen G</t>
-  </si>
-  <si>
-    <t>Theater</t>
-  </si>
-  <si>
-    <t>Ian I</t>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Cat C</t>
+  </si>
+  <si>
+    <t>David D</t>
   </si>
   <si>
     <t>No Preference</t>
-  </si>
-  <si>
-    <t>Tony J</t>
-  </si>
-  <si>
-    <t>Karch K</t>
-  </si>
-  <si>
-    <t>Dance</t>
-  </si>
-  <si>
-    <t>Ben C</t>
-  </si>
-  <si>
-    <t>Dan L</t>
-  </si>
-  <si>
-    <t>Cat J</t>
-  </si>
-  <si>
-    <t>Jon M</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Mengchen Gong</t>
-  </si>
-  <si>
-    <t>Laila L</t>
   </si>
 </sst>
 </file>
@@ -417,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,10 +438,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -473,13 +449,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -490,108 +466,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>